<commit_message>
working on template upload
</commit_message>
<xml_diff>
--- a/server/content/templates/Linear Regression.xlsx
+++ b/server/content/templates/Linear Regression.xlsx
@@ -24,14 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>x 
-(independent variable)</t>
+    <t xml:space="preserve">x </t>
   </si>
   <si>
-    <t>y 
-(dependent variable)</t>
+    <t>(independent variable)</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>(dependent variable)</t>
   </si>
 </sst>
 </file>
@@ -377,10 +381,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -388,15 +392,24 @@
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
built initial persistance in mongo DB and redirect based on the DB id
</commit_message>
<xml_diff>
--- a/server/content/templates/Linear Regression.xlsx
+++ b/server/content/templates/Linear Regression.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">x </t>
-  </si>
-  <si>
     <t>(independent variable)</t>
   </si>
   <si>
@@ -36,6 +33,9 @@
   </si>
   <si>
     <t>(dependent variable)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,18 +398,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>